<commit_message>
feat: a whole lot
</commit_message>
<xml_diff>
--- a/goal-demo-schedule.xlsx
+++ b/goal-demo-schedule.xlsx
@@ -46,13 +46,13 @@
     <t xml:space="preserve">Lecturer</t>
   </si>
   <si>
-    <t xml:space="preserve">Johnson</t>
+    <t xml:space="preserve">Winchester</t>
   </si>
   <si>
     <t xml:space="preserve">Course</t>
   </si>
   <si>
-    <t xml:space="preserve">7C</t>
+    <t xml:space="preserve">A8</t>
   </si>
   <si>
     <t xml:space="preserve">0 – Wednesday</t>
@@ -474,10 +474,10 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.4296875" defaultRowHeight="36" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.4375" defaultRowHeight="36" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="41.13"/>

</xml_diff>